<commit_message>
other test classes adde
</commit_message>
<xml_diff>
--- a/src/test/java/test_data/BookingFlight.xlsx
+++ b/src/test/java/test_data/BookingFlight.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milosvajagic/IdeaProjects/BookingFlight/src/test/java/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B3683F-C527-6B43-B4D3-73F3055A8847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D124D734-D40A-3849-BA7D-3CEFAF8B1837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="19860" xr2:uid="{11A8D5B1-71A7-4F44-AA83-BC060844EF71}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{11A8D5B1-71A7-4F44-AA83-BC060844EF71}"/>
   </bookViews>
   <sheets>
     <sheet name="BookingSheetFlight" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Flight Page</t>
   </si>
@@ -53,23 +53,55 @@
     <t>Budapest</t>
   </si>
   <si>
-    <t>2022-02-25</t>
-  </si>
-  <si>
     <t>Belgrade</t>
   </si>
   <si>
-    <t>2022-02-27</t>
+    <t>2022-03-03</t>
+  </si>
+  <si>
+    <t>2022-03-27</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>milosmarkovic@test.com</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Milos</t>
+  </si>
+  <si>
+    <t>Markovic</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,17 +124,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -415,27 +453,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81BC9A60-03DB-6244-9C06-B502F2C064E6}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -448,25 +488,53 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{C0296577-1873-ED4C-9B6B-D2E9250B28CA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
appropriate selectors are added
</commit_message>
<xml_diff>
--- a/src/test/java/test_data/BookingFlight.xlsx
+++ b/src/test/java/test_data/BookingFlight.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milosvajagic/IdeaProjects/BookingFlight/src/test/java/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9FB52C-945F-1848-AA3E-A92B9A9458E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089540DE-D576-884D-BDAB-8B1C84F7F2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{11A8D5B1-71A7-4F44-AA83-BC060844EF71}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{11A8D5B1-71A7-4F44-AA83-BC060844EF71}"/>
   </bookViews>
   <sheets>
     <sheet name="BookingSheetFlight" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Flight Page</t>
   </si>
@@ -90,6 +90,30 @@
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t>Vienna</t>
+  </si>
+  <si>
+    <t>2022-03-05</t>
+  </si>
+  <si>
+    <t>2022-03-08</t>
+  </si>
+  <si>
+    <t>vesna92@test.com</t>
+  </si>
+  <si>
+    <t>Vesna</t>
+  </si>
+  <si>
+    <t>Todoric</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>63522526</t>
   </si>
 </sst>
 </file>
@@ -460,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81BC9A60-03DB-6244-9C06-B502F2C064E6}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,12 +564,42 @@
         <v>17</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{C0296577-1873-ED4C-9B6B-D2E9250B28CA}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{B8354B27-6806-5C4F-BD12-3013369F90FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>